<commit_message>
consultas sql y tareas agregadas a modulos
</commit_message>
<xml_diff>
--- a/SPRINT 1/CRONOGRAMA VERSUS 2.xlsx
+++ b/SPRINT 1/CRONOGRAMA VERSUS 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adela\OneDrive\Documentos\RESIDENCIA\FarmaciaGiDocumentos\SPRINT 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/73a9b2cc98479d66/Documentos/RESIDENCIA/FarmaciaGiDocumentos/SPRINT 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E31CF26-E137-4AA8-A5D4-FFC1CDFBF15C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="888" documentId="13_ncr:1_{6A2C58A2-E982-43E3-AFBE-98355306293A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1430A37A-8029-4387-B651-D6CDF7C1315F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{DD5450A7-52F7-4CDB-9166-D906894400A3}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="893" uniqueCount="495">
   <si>
     <t>Sprint</t>
   </si>
@@ -1529,87 +1529,6 @@
   </si>
   <si>
     <t>Precio sin punto</t>
-  </si>
-  <si>
-    <t>corregir existencias</t>
-  </si>
-  <si>
-    <t>corregir insertar productos  por codigo de barras y o nombre error</t>
-  </si>
-  <si>
-    <t>corregir formato de corte de caja</t>
-  </si>
-  <si>
-    <t>terminar reportes diarios como lo quiere la doctora</t>
-  </si>
-  <si>
-    <t>orregir reporte de inventario: solo funciona con salidas</t>
-  </si>
-  <si>
-    <t>terminar los terminos ya agregados en marco teorico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">estructurar desarrollo en la documentacion </t>
-  </si>
-  <si>
-    <t>complementar manual de usuario</t>
-  </si>
-  <si>
-    <t>darle responsibidad a vistas del ecomerce</t>
-  </si>
-  <si>
-    <t>impresión directo del ticket</t>
-  </si>
-  <si>
-    <t>vistas de seguimiento de pedido</t>
-  </si>
-  <si>
-    <t>terminar pagos contraentrega</t>
-  </si>
-  <si>
-    <t>pagos paypal</t>
-  </si>
-  <si>
-    <t>vistas del modulo de cotizacion</t>
-  </si>
-  <si>
-    <t>FOTO PERSONAL PANORAMICA: img_1220</t>
-  </si>
-  <si>
-    <t>INDIVIDUAL PARA AGRADECIEMNTO. IMG_1221</t>
-  </si>
-  <si>
-    <t>FOTO FAMILAIR</t>
-  </si>
-  <si>
-    <t>FOTO DE RELAJO</t>
-  </si>
-  <si>
-    <t>INDIVIDUAL REGALIA</t>
-  </si>
-  <si>
-    <t>fotomontaje para familiar</t>
-  </si>
-  <si>
-    <t>carrera</t>
-  </si>
-  <si>
-    <t>confirmar correo de los clientes que se registran en el ecommerce</t>
-  </si>
-  <si>
-    <t>testear envios de correos del modulo monitoreo</t>
-  </si>
-  <si>
-    <t>cargar bd de pruebas y respaldar para trabajar sobre eso</t>
-  </si>
-  <si>
-    <t>checar las fechas de caducidad no los guardo : error fehcas de caducidad</t>
-  </si>
-  <si>
-    <t>tener 10 valores diferentes para las pruebas</t>
-  </si>
-  <si>
-    <t>** probar una vez cargados nuevos datos</t>
   </si>
 </sst>
 </file>
@@ -6404,14 +6323,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{389771CD-3F00-45C6-928B-7954571D8EB7}">
   <dimension ref="A1:O201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="44.42578125" customWidth="1"/>
-    <col min="5" max="5" width="49.42578125" customWidth="1"/>
+    <col min="5" max="5" width="105.42578125" customWidth="1"/>
     <col min="13" max="13" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6601,9 +6520,6 @@
       <c r="A17" t="s">
         <v>325</v>
       </c>
-      <c r="D17" t="s">
-        <v>495</v>
-      </c>
       <c r="M17" t="s">
         <v>265</v>
       </c>
@@ -6612,12 +6528,6 @@
       <c r="A18" t="s">
         <v>326</v>
       </c>
-      <c r="D18" t="s">
-        <v>496</v>
-      </c>
-      <c r="F18" t="s">
-        <v>521</v>
-      </c>
       <c r="M18" t="s">
         <v>418</v>
       </c>
@@ -6626,9 +6536,6 @@
       <c r="A19" t="s">
         <v>351</v>
       </c>
-      <c r="D19" t="s">
-        <v>497</v>
-      </c>
       <c r="M19" t="s">
         <v>424</v>
       </c>
@@ -6637,9 +6544,6 @@
       <c r="A20" t="s">
         <v>373</v>
       </c>
-      <c r="D20" t="s">
-        <v>499</v>
-      </c>
       <c r="M20" t="s">
         <v>426</v>
       </c>
@@ -6648,9 +6552,6 @@
       <c r="A21" t="s">
         <v>410</v>
       </c>
-      <c r="D21" t="s">
-        <v>498</v>
-      </c>
       <c r="M21" t="s">
         <v>427</v>
       </c>
@@ -6659,9 +6560,6 @@
       <c r="A22" t="s">
         <v>413</v>
       </c>
-      <c r="D22" t="s">
-        <v>500</v>
-      </c>
       <c r="M22" t="s">
         <v>428</v>
       </c>
@@ -6670,9 +6568,6 @@
       <c r="A23" t="s">
         <v>435</v>
       </c>
-      <c r="D23" t="s">
-        <v>501</v>
-      </c>
       <c r="M23" t="s">
         <v>429</v>
       </c>
@@ -6681,9 +6576,6 @@
       <c r="A24" t="s">
         <v>327</v>
       </c>
-      <c r="D24" t="s">
-        <v>502</v>
-      </c>
       <c r="M24" t="s">
         <v>430</v>
       </c>
@@ -6692,9 +6584,6 @@
       <c r="A25" t="s">
         <v>328</v>
       </c>
-      <c r="D25" t="s">
-        <v>504</v>
-      </c>
       <c r="M25" t="s">
         <v>242</v>
       </c>
@@ -6703,9 +6592,6 @@
       <c r="A26" t="s">
         <v>329</v>
       </c>
-      <c r="D26" t="s">
-        <v>503</v>
-      </c>
       <c r="M26" t="s">
         <v>264</v>
       </c>
@@ -6714,9 +6600,6 @@
       <c r="A27" t="s">
         <v>378</v>
       </c>
-      <c r="D27" t="s">
-        <v>519</v>
-      </c>
       <c r="M27" t="s">
         <v>245</v>
       </c>
@@ -6725,9 +6608,6 @@
       <c r="A28" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="D28" t="s">
-        <v>505</v>
-      </c>
       <c r="M28" t="s">
         <v>282</v>
       </c>
@@ -6736,9 +6616,6 @@
       <c r="A29" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="D29" t="s">
-        <v>506</v>
-      </c>
       <c r="M29" t="s">
         <v>272</v>
       </c>
@@ -6747,9 +6624,6 @@
       <c r="A30" s="23" t="s">
         <v>247</v>
       </c>
-      <c r="D30" t="s">
-        <v>507</v>
-      </c>
       <c r="M30" t="s">
         <v>286</v>
       </c>
@@ -6758,9 +6632,6 @@
       <c r="A31" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D31" t="s">
-        <v>508</v>
-      </c>
       <c r="M31" t="s">
         <v>287</v>
       </c>
@@ -6769,9 +6640,6 @@
       <c r="A32" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="D32" t="s">
-        <v>516</v>
-      </c>
       <c r="M32" t="s">
         <v>288</v>
       </c>
@@ -6780,9 +6648,6 @@
       <c r="A33" t="s">
         <v>291</v>
       </c>
-      <c r="D33" t="s">
-        <v>517</v>
-      </c>
       <c r="M33" t="s">
         <v>289</v>
       </c>
@@ -6791,9 +6656,6 @@
       <c r="A34" t="s">
         <v>457</v>
       </c>
-      <c r="D34" t="s">
-        <v>518</v>
-      </c>
       <c r="M34" t="s">
         <v>269</v>
       </c>
@@ -6802,9 +6664,6 @@
       <c r="A35" t="s">
         <v>441</v>
       </c>
-      <c r="D35" t="s">
-        <v>520</v>
-      </c>
       <c r="M35" t="s">
         <v>285</v>
       </c>
@@ -6842,62 +6701,36 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>509</v>
-      </c>
       <c r="M40" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>510</v>
-      </c>
       <c r="M41" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>511</v>
-      </c>
       <c r="M42" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>512</v>
-      </c>
       <c r="M43" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>513</v>
-      </c>
       <c r="M44" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>9512861203</v>
-      </c>
       <c r="M45" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>514</v>
-      </c>
-    </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>515</v>
-      </c>
       <c r="M47" t="s">
         <v>204</v>
       </c>

</xml_diff>